<commit_message>
update pour la second round, quelques changements
</commit_message>
<xml_diff>
--- a/excel/tourner-dans-le-vide.xlsx
+++ b/excel/tourner-dans-le-vide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remilevesque/foot2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4542C11E-1610-6F49-8448-278E9CD59A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD8E0C7-F0B4-034E-9600-4F717F1BE5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="127">
   <si>
     <t>Timestamp</t>
   </si>
@@ -296,6 +296,111 @@
   </si>
   <si>
     <t>Doudou</t>
+  </si>
+  <si>
+    <t>Jaguars vs Chiefs</t>
+  </si>
+  <si>
+    <t>Jaguars vs Chiefs Score</t>
+  </si>
+  <si>
+    <t>Jaguars vs Chiefs Over Under (53)</t>
+  </si>
+  <si>
+    <t>Giants vs Eagles</t>
+  </si>
+  <si>
+    <t>Giants vs Eagles Score</t>
+  </si>
+  <si>
+    <t>Giants vs Eagles Over Under (48)</t>
+  </si>
+  <si>
+    <t>Bengals vs Bills</t>
+  </si>
+  <si>
+    <t>Bengals vs Bills Score</t>
+  </si>
+  <si>
+    <t>Bengals vs Bills Over Under (49)</t>
+  </si>
+  <si>
+    <t>Cowboys vs Niners</t>
+  </si>
+  <si>
+    <t>Cowboys vs Niners Score</t>
+  </si>
+  <si>
+    <t>Cowboys vs Niners Over Under (46)</t>
+  </si>
+  <si>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>31 à 17</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>31 à 24</t>
+  </si>
+  <si>
+    <t>27 à 21</t>
+  </si>
+  <si>
+    <t>35-20 Chiefs</t>
+  </si>
+  <si>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>27-20 Eagles</t>
+  </si>
+  <si>
+    <t>35-31 Bengals</t>
+  </si>
+  <si>
+    <t>27-14 Niners</t>
+  </si>
+  <si>
+    <t>38-35</t>
+  </si>
+  <si>
+    <t>30-18</t>
+  </si>
+  <si>
+    <t>30-17</t>
+  </si>
+  <si>
+    <t>28-17</t>
+  </si>
+  <si>
+    <t>26-18</t>
+  </si>
+  <si>
+    <t>35-21</t>
+  </si>
+  <si>
+    <t>30-24</t>
+  </si>
+  <si>
+    <t>30-13</t>
+  </si>
+  <si>
+    <t>30-20</t>
+  </si>
+  <si>
+    <t>35-27</t>
+  </si>
+  <si>
+    <t>31-21</t>
+  </si>
+  <si>
+    <t>34-27</t>
+  </si>
+  <si>
+    <t>23-20</t>
   </si>
 </sst>
 </file>
@@ -320,11 +425,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -351,10 +456,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,42 +676,51 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="19.5" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="44.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" customWidth="1"/>
-    <col min="9" max="9" width="30.1640625" customWidth="1"/>
-    <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" customWidth="1"/>
-    <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" customWidth="1"/>
-    <col min="15" max="15" width="26.1640625" customWidth="1"/>
-    <col min="16" max="16" width="15.1640625" customWidth="1"/>
-    <col min="17" max="17" width="20.1640625" customWidth="1"/>
-    <col min="18" max="18" width="29.1640625" customWidth="1"/>
-    <col min="19" max="19" width="15" customWidth="1"/>
-    <col min="20" max="20" width="19.6640625" customWidth="1"/>
-    <col min="21" max="21" width="28.83203125" customWidth="1"/>
-    <col min="22" max="22" width="22" customWidth="1"/>
-    <col min="23" max="23" width="22.6640625" customWidth="1"/>
-    <col min="24" max="29" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,10 +784,44 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
+      <c r="V1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>44940.491280011571</v>
       </c>
@@ -739,10 +885,44 @@
       <c r="U2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
+      <c r="V2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>44940.316606215274</v>
       </c>
@@ -806,10 +986,44 @@
       <c r="U3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
+      <c r="V3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>44940.704032928239</v>
       </c>
@@ -873,10 +1087,44 @@
       <c r="U4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
+      <c r="V4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>45227</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>44940.63775991898</v>
       </c>
@@ -940,9 +1188,44 @@
       <c r="U5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="W5" s="1"/>
+      <c r="V5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>44940.479377314812</v>
       </c>
@@ -1006,9 +1289,44 @@
       <c r="U6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="W6" s="1"/>
+      <c r="V6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>44940.662635416666</v>
       </c>
@@ -1072,10 +1390,44 @@
       <c r="U7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V7" s="3"/>
-      <c r="W7" s="1"/>
+      <c r="V7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG7" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>44939.676858773149</v>
       </c>
@@ -1139,10 +1491,44 @@
       <c r="U8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
+      <c r="V8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG8" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>44940.376684062503</v>
       </c>
@@ -1206,10 +1592,44 @@
       <c r="U9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
+      <c r="V9" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG9" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>44939.934279189816</v>
       </c>
@@ -1273,8 +1693,42 @@
       <c r="U10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V10" s="4"/>
-      <c r="W10" s="1"/>
+      <c r="V10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF10" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG10" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>